<commit_message>
Adding the More Test Case
</commit_message>
<xml_diff>
--- a/testData/Opencart_LoginData.xlsx
+++ b/testData/Opencart_LoginData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sangram.magdum\Desktop\New folder\HybridFrameWork\openCart\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B63A7FD-588E-4927-8698-D6D943432410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFB1F4C-F942-4928-BB21-9557F5D8BECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23740" yWindow="5050" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24970" yWindow="5730" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -46,6 +46,21 @@
   </si>
   <si>
     <t>smith@fakemail.com</t>
+  </si>
+  <si>
+    <t>MikeS@78</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>MikeS@</t>
+  </si>
+  <si>
+    <t>michael@fakemail.com</t>
+  </si>
+  <si>
+    <t>MikeS</t>
   </si>
 </sst>
 </file>
@@ -377,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -415,12 +430,44 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{B90070E4-862E-4C58-B646-8FDFAC8F9EED}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{E98C2AEA-4EFB-4D87-B146-56EDBCCFA198}"/>
     <hyperlink ref="A3" r:id="rId3" xr:uid="{33333352-6C74-4D33-8AF5-1E6436AE1D32}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{D888AB24-A07C-449B-BEC8-540ADBA72BEB}"/>
+    <hyperlink ref="B4" r:id="rId5" display="MikeS@78" xr:uid="{102397B5-D157-4927-9B52-3C8D94105D2A}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{0006B8A3-9886-4FD3-932C-9DEEF62ACA79}"/>
+    <hyperlink ref="A5" r:id="rId7" xr:uid="{B5AFF3CA-CBD6-4143-9CA5-577A8C8E35E4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>